<commit_message>
add number and fix bug edit sales
</commit_message>
<xml_diff>
--- a/assets/excel/Data Inquiry.xlsx
+++ b/assets/excel/Data Inquiry.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
   <si>
     <t>ID Inquiry</t>
   </si>
@@ -134,6 +134,36 @@
     <t>EUR</t>
   </si>
   <si>
+    <t xml:space="preserve">IT </t>
+  </si>
+  <si>
+    <t>2021-09-07 13:12:27</t>
+  </si>
+  <si>
+    <t>EATON</t>
+  </si>
+  <si>
+    <t>eaton serie xxxxxx</t>
+  </si>
+  <si>
+    <t>2021-09-07</t>
+  </si>
+  <si>
+    <t>yeyeye</t>
+  </si>
+  <si>
+    <t>2021-09-07 13:20:49</t>
+  </si>
+  <si>
+    <t>sgd</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAYENTI </t>
+  </si>
+  <si>
     <t>2021-09-02 13:43:12</t>
   </si>
   <si>
@@ -179,15 +209,33 @@
     <t>23 WEEKS</t>
   </si>
   <si>
+    <t>2021-09-03 11:17:24</t>
+  </si>
+  <si>
+    <t>NACOL</t>
+  </si>
+  <si>
+    <t>tttt</t>
+  </si>
+  <si>
+    <t>2021-09-03</t>
+  </si>
+  <si>
+    <t>tested</t>
+  </si>
+  <si>
+    <t>PRICE+LT</t>
+  </si>
+  <si>
+    <t>2021-09-06 16:46:12</t>
+  </si>
+  <si>
     <t>2021-09-03 14:03:24</t>
   </si>
   <si>
     <t>A244343DFDF</t>
   </si>
   <si>
-    <t>2021-09-03</t>
-  </si>
-  <si>
     <t xml:space="preserve">TEST TEST TEST TEST TEST TEST </t>
   </si>
   <si>
@@ -216,9 +264,6 @@
   </si>
   <si>
     <t>2021-09-14</t>
-  </si>
-  <si>
-    <t>PRICE+LT</t>
   </si>
   <si>
     <t>2021-09-06 14:58:23</t>
@@ -563,7 +608,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -759,185 +804,185 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4">
-        <v>18733</v>
+        <v>18732</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="M4">
-        <v>111</v>
+        <v>0.003</v>
       </c>
       <c r="N4" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="O4">
-        <v>2132323</v>
+        <v>10000</v>
       </c>
       <c r="P4">
-        <v>1212121</v>
+        <v>100000</v>
       </c>
       <c r="Q4">
-        <v>121212</v>
+        <v>100000</v>
       </c>
       <c r="R4">
-        <v>12121</v>
+        <v>100000</v>
       </c>
       <c r="S4" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="T4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5">
-        <v>18734</v>
+        <v>18733</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
         <v>36</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="L5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="N5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="O5">
-        <v>212</v>
+        <v>2132323</v>
       </c>
       <c r="P5">
-        <v>111</v>
+        <v>1212121</v>
       </c>
       <c r="Q5">
-        <v>222</v>
+        <v>121212</v>
       </c>
       <c r="R5">
-        <v>1112</v>
+        <v>12121</v>
       </c>
       <c r="S5" t="s">
-        <v>53</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="T5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6">
-        <v>18736</v>
+        <v>18734</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M6">
-        <v>121.232</v>
+        <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="O6">
-        <v>232323</v>
+        <v>212</v>
       </c>
       <c r="P6">
-        <v>2323232</v>
+        <v>111</v>
       </c>
       <c r="Q6">
-        <v>12121</v>
+        <v>222</v>
       </c>
       <c r="R6">
-        <v>121232</v>
+        <v>1112</v>
       </c>
       <c r="S6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="T6">
         <v>1</v>
@@ -945,63 +990,187 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7">
+        <v>18735</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7">
+        <v>23223.131</v>
+      </c>
+      <c r="N7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7">
+        <v>12324</v>
+      </c>
+      <c r="P7">
+        <v>2232323</v>
+      </c>
+      <c r="Q7">
+        <v>1212121</v>
+      </c>
+      <c r="R7">
+        <v>121212</v>
+      </c>
+      <c r="S7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8">
+        <v>18736</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8">
+        <v>121.232</v>
+      </c>
+      <c r="N8" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8">
+        <v>232323</v>
+      </c>
+      <c r="P8">
+        <v>2323232</v>
+      </c>
+      <c r="Q8">
+        <v>12121</v>
+      </c>
+      <c r="R8">
+        <v>121232</v>
+      </c>
+      <c r="S8" t="s">
+        <v>77</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9">
         <v>18737</v>
       </c>
-      <c r="B7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7">
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9">
         <v>2</v>
       </c>
-      <c r="G7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>68</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="G9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" t="s">
         <v>25</v>
       </c>
-      <c r="M7">
+      <c r="M9">
         <v>200</v>
       </c>
-      <c r="N7" t="s">
-        <v>60</v>
-      </c>
-      <c r="O7">
+      <c r="N9" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9">
         <v>200000</v>
       </c>
-      <c r="P7">
+      <c r="P9">
         <v>2002020</v>
       </c>
-      <c r="Q7">
+      <c r="Q9">
         <v>2000000</v>
       </c>
-      <c r="R7">
+      <c r="R9">
         <v>2000000</v>
       </c>
-      <c r="S7" t="s">
-        <v>69</v>
-      </c>
-      <c r="T7"/>
+      <c r="S9" t="s">
+        <v>84</v>
+      </c>
+      <c r="T9"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
fix ui and add new table pharsing
</commit_message>
<xml_diff>
--- a/assets/excel/Data Inquiry.xlsx
+++ b/assets/excel/Data Inquiry.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
   <si>
     <t>ID Inquiry</t>
   </si>
@@ -104,7 +104,7 @@
     <t>tetete</t>
   </si>
   <si>
-    <t>EURO</t>
+    <t>EUR</t>
   </si>
   <si>
     <t>18 weeks</t>
@@ -113,7 +113,7 @@
     <t>2021-09-01 09:52:22</t>
   </si>
   <si>
-    <t>EATON AIRFLEX</t>
+    <t>EATON</t>
   </si>
   <si>
     <t>DDSDSD2</t>
@@ -131,15 +131,9 @@
     <t>aaaaa</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>2021-09-01 10:08:26</t>
   </si>
   <si>
-    <t>EATON JEIL</t>
-  </si>
-  <si>
     <t>TEEWRERE</t>
   </si>
   <si>
@@ -158,9 +152,6 @@
     <t>2021-09-01 10:08:58</t>
   </si>
   <si>
-    <t>EATON AEROQUIP</t>
-  </si>
-  <si>
     <t>testtt</t>
   </si>
   <si>
@@ -179,9 +170,6 @@
     <t>2021-09-01 13:48:46</t>
   </si>
   <si>
-    <t>EATON MOELLER</t>
-  </si>
-  <si>
     <t>sfaasdsd</t>
   </si>
   <si>
@@ -194,15 +182,9 @@
     <t>ok</t>
   </si>
   <si>
-    <t>Euro</t>
-  </si>
-  <si>
     <t>2021-09-07 13:12:27</t>
   </si>
   <si>
-    <t>EATON</t>
-  </si>
-  <si>
     <t>eaton serie xxxxxx</t>
   </si>
   <si>
@@ -215,9 +197,6 @@
     <t>2021-09-07 13:20:49</t>
   </si>
   <si>
-    <t>sgd</t>
-  </si>
-  <si>
     <t xml:space="preserve">MAYENTI </t>
   </si>
   <si>
@@ -245,9 +224,6 @@
     <t>2021-09-02 16:35:55</t>
   </si>
   <si>
-    <t>INTEGRAL</t>
-  </si>
-  <si>
     <t>a343trer34f</t>
   </si>
   <si>
@@ -293,7 +269,7 @@
     <t>wwwww</t>
   </si>
   <si>
-    <t>Jpy</t>
+    <t>JPY</t>
   </si>
   <si>
     <t>18 Hour</t>
@@ -318,6 +294,21 @@
   </si>
   <si>
     <t>14 hari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADMIN </t>
+  </si>
+  <si>
+    <t>2021-09-10 15:17:52</t>
+  </si>
+  <si>
+    <t>kekei</t>
+  </si>
+  <si>
+    <t>2021-09-11 09:04:21</t>
+  </si>
+  <si>
+    <t>21 Weeks</t>
   </si>
 </sst>
 </file>
@@ -656,7 +647,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -829,10 +820,10 @@
         <v>12121.102</v>
       </c>
       <c r="N3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="O3">
-        <v>212232323</v>
+        <v>134544227</v>
       </c>
       <c r="P3">
         <v>23223232</v>
@@ -858,13 +849,13 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
         <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -876,13 +867,13 @@
         <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L4" t="s">
         <v>37</v>
@@ -891,7 +882,7 @@
         <v>222.22</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O4">
         <v>1111</v>
@@ -909,7 +900,7 @@
         <v>11111</v>
       </c>
       <c r="T4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -920,13 +911,13 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -944,16 +935,16 @@
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M5">
         <v>12121.1</v>
       </c>
       <c r="N5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O5">
         <v>2323</v>
@@ -968,10 +959,10 @@
         <v>1212121</v>
       </c>
       <c r="S5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="T5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -982,13 +973,13 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -997,7 +988,7 @@
         <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I6" t="s">
         <v>36</v>
@@ -1006,16 +997,16 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M6">
         <v>1222.121</v>
       </c>
       <c r="N6" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -1033,7 +1024,7 @@
         <v>30</v>
       </c>
       <c r="T6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -1041,25 +1032,25 @@
         <v>18732</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I7" t="s">
         <v>26</v>
@@ -1068,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="L7" t="s">
         <v>25</v>
@@ -1077,7 +1068,7 @@
         <v>0.003</v>
       </c>
       <c r="N7" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="O7">
         <v>10000</v>
@@ -1092,10 +1083,10 @@
         <v>100000</v>
       </c>
       <c r="S7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -1106,22 +1097,22 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I8" t="s">
         <v>36</v>
@@ -1130,10 +1121,10 @@
         <v>2</v>
       </c>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="L8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="M8">
         <v>111</v>
@@ -1157,7 +1148,7 @@
         <v>30</v>
       </c>
       <c r="T8" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1168,22 +1159,22 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" t="s">
         <v>70</v>
-      </c>
-      <c r="H9" t="s">
-        <v>78</v>
       </c>
       <c r="I9" t="s">
         <v>36</v>
@@ -1192,16 +1183,16 @@
         <v>6</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="L9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="M9">
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="O9">
         <v>212</v>
@@ -1216,7 +1207,7 @@
         <v>1112</v>
       </c>
       <c r="S9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="T9">
         <v>1</v>
@@ -1230,34 +1221,34 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="L10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="M10">
         <v>23223.131</v>
@@ -1278,10 +1269,10 @@
         <v>121212</v>
       </c>
       <c r="S10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="T10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1292,22 +1283,22 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H11" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="I11" t="s">
         <v>26</v>
@@ -1316,16 +1307,16 @@
         <v>2</v>
       </c>
       <c r="K11" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="L11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="M11">
         <v>121.232</v>
       </c>
       <c r="N11" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="O11">
         <v>232323</v>
@@ -1340,7 +1331,7 @@
         <v>121232</v>
       </c>
       <c r="S11" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="T11">
         <v>1</v>
@@ -1351,34 +1342,34 @@
         <v>18737</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H12" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I12" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="L12" t="s">
         <v>25</v>
@@ -1387,7 +1378,7 @@
         <v>200</v>
       </c>
       <c r="N12" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="O12">
         <v>200000</v>
@@ -1402,9 +1393,69 @@
         <v>2000000</v>
       </c>
       <c r="S12" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="T12"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13">
+        <v>18738</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>96</v>
+      </c>
+      <c r="L13"/>
+      <c r="M13">
+        <v>112.221</v>
+      </c>
+      <c r="N13" t="s">
+        <v>42</v>
+      </c>
+      <c r="O13">
+        <v>1627205</v>
+      </c>
+      <c r="P13">
+        <v>2928969</v>
+      </c>
+      <c r="Q13">
+        <v>3091689</v>
+      </c>
+      <c r="R13">
+        <v>3254410</v>
+      </c>
+      <c r="S13" t="s">
+        <v>97</v>
+      </c>
+      <c r="T13" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>